<commit_message>
schedule validate on create and  drop down complete, fixing notification emails on change by user
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>id</t>
   </si>
@@ -29,7 +29,13 @@
     <t>role_id</t>
   </si>
   <si>
-    <t> </t>
+    <t>batch_id</t>
+  </si>
+  <si>
+    <t>semester_id</t>
+  </si>
+  <si>
+    <t>branch_id</t>
   </si>
   <si>
     <t>Akshita Pradhan</t>
@@ -166,10 +172,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -178,7 +184,8 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4489795918367"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.030612244898"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.05612244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="21.2551020408163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.43877551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.8061224489796"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -199,7 +206,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -207,12 +217,21 @@
         <v>12070121701</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="0" t="n">
         <v>3</v>
       </c>
     </row>
@@ -221,13 +240,22 @@
         <v>12070121113</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>3</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -235,13 +263,22 @@
         <v>12070121102</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create single user and send mails on change complete
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -38,10 +38,10 @@
     <t>branch_id</t>
   </si>
   <si>
-    <t>Akshita Pradhan</t>
-  </si>
-  <si>
-    <t>akshita.pradhan@sitpune.edu.in</t>
+    <t>Mehul Chopda</t>
+  </si>
+  <si>
+    <t>mehul.chopda@sitpune.edu.in</t>
   </si>
   <si>
     <t>Dibyajyoti Ghosh</t>
@@ -50,10 +50,10 @@
     <t>ghoshdibya05@gmail.com</t>
   </si>
   <si>
-    <t>Aishwarya Singh</t>
-  </si>
-  <si>
-    <t>aishwarya.singh@sitpune.edu.in</t>
+    <t>Abhiraj Bishnoi</t>
+  </si>
+  <si>
+    <t>abhiraj.bishnoi@sitpune.edu.in</t>
   </si>
 </sst>
 </file>
@@ -175,7 +175,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -272,7 +272,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>5</v>
@@ -283,9 +283,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="akshita.pradhan@sitpune.edu.in"/>
-    <hyperlink ref="C3" r:id="rId2" display="ghoshdibya05@gmail.com"/>
-    <hyperlink ref="C4" r:id="rId3" display="aishwarya.singh@sitpune.edu.in"/>
+    <hyperlink ref="C3" r:id="rId1" display="ghoshdibya05@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
removed all js from manifest
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -175,7 +175,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -214,7 +214,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>12070121701</v>
+        <v>701</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>7</v>
@@ -237,7 +237,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>12070121113</v>
+        <v>113</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>9</v>
@@ -260,7 +260,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>12070121102</v>
+        <v>602</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Changed CSS, Import error display not Working
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -175,7 +175,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -229,7 +229,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>3</v>
@@ -252,7 +252,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>1</v>
@@ -275,7 +275,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Displaying excel error messages
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>id</t>
   </si>
@@ -36,6 +36,12 @@
   </si>
   <si>
     <t>branch_id</t>
+  </si>
+  <si>
+    <t>Aishwarya Singh</t>
+  </si>
+  <si>
+    <t>1994aishwaryasingh@gmail.com</t>
   </si>
   <si>
     <t>Mehul Chopda</t>
@@ -63,7 +69,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -91,6 +97,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF3C3C3C"/>
+      <name val="Ubuntu"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -142,7 +154,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -152,6 +164,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -164,6 +180,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF3C3C3C"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -172,10 +248,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -212,9 +288,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>701</v>
+        <v>1102</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>7</v>
@@ -232,17 +308,17 @@
         <v>6</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>113</v>
+        <v>701</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="0" t="n">
@@ -255,35 +331,59 @@
         <v>6</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>602</v>
+        <v>113</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>602</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="G4" s="0" t="n">
+      <c r="E5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G5" s="0" t="n">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" display="ghoshdibya05@gmail.com"/>
+    <hyperlink ref="C2" r:id="rId1" display="1994aishwaryasingh@gmail.com"/>
+    <hyperlink ref="C4" r:id="rId2" display="ghoshdibya05@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
email not working again, and email not correctly validated
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -38,28 +38,28 @@
     <t>branch_id</t>
   </si>
   <si>
-    <t>Aishwarya Singh</t>
-  </si>
-  <si>
-    <t>1994aishwaryasingh@gmail.com</t>
-  </si>
-  <si>
     <t>Mehul Chopda</t>
   </si>
   <si>
     <t>mehul.chopda@sitpune.edu.in</t>
   </si>
   <si>
-    <t>Dibyajyoti Ghosh</t>
-  </si>
-  <si>
-    <t>ghoshdibya05@gmail.com</t>
-  </si>
-  <si>
     <t>Abhiraj Bishnoi</t>
   </si>
   <si>
     <t>abhiraj.bishnoi@sitpune.edu.in</t>
+  </si>
+  <si>
+    <t>Aishwarya Singh Bhati</t>
+  </si>
+  <si>
+    <t>aishwarya.singh@sitpune.edu.in</t>
+  </si>
+  <si>
+    <t>Akshita Pradhan</t>
+  </si>
+  <si>
+    <t>akshita.pradhan@sitpune.edu.in</t>
   </si>
 </sst>
 </file>
@@ -69,7 +69,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -97,12 +97,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF3C3C3C"/>
-      <name val="Ubuntu"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -154,7 +148,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -167,10 +161,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -180,66 +170,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF3C3C3C"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -251,7 +181,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -288,9 +218,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1102</v>
+        <v>701</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>7</v>
@@ -308,82 +238,64 @@
         <v>6</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>701</v>
+        <v>602</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>6</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>113</v>
+        <v>135</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>3</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>602</v>
+        <v>790</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="1994aishwaryasingh@gmail.com"/>
-    <hyperlink ref="C4" r:id="rId2" display="ghoshdibya05@gmail.com"/>
+    <hyperlink ref="C4" r:id="rId1" display="aishwarya.singh@sitpune.edu.in"/>
+    <hyperlink ref="C5" r:id="rId2" display="akshita.pradhan@sitpune.edu.in"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
email validation and other validation on importing the excel sheet added.
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -60,6 +60,18 @@
   </si>
   <si>
     <t>akshita.pradhan@sitpune.edu.in</t>
+  </si>
+  <si>
+    <t>Ameya Bhattacharya</t>
+  </si>
+  <si>
+    <t>ameya.bhattacharya@sitpune.edu.in</t>
+  </si>
+  <si>
+    <t>Aishwarya Singh</t>
+  </si>
+  <si>
+    <t>1994aishwaryasingh@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -178,17 +190,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.780612244898"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4489795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.030612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.2244897959184"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.05612244897959"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.43877551020408"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.8061224489796"/>
@@ -277,6 +289,15 @@
       <c r="D4" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="E4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -290,12 +311,51 @@
       </c>
       <c r="D5" s="0" t="n">
         <v>3</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5678</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" display="aishwarya.singh@sitpune.edu.in"/>
     <hyperlink ref="C5" r:id="rId2" display="akshita.pradhan@sitpune.edu.in"/>
+    <hyperlink ref="C6" r:id="rId3" display="ameya.bhattacharya@sitpune.edu.in"/>
+    <hyperlink ref="C7" r:id="rId4" display="1994aishwaryasingh@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
changed roke_id validation on import
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="223" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>id</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>1994aishwaryasingh@gmail.com</t>
+  </si>
+  <si>
+    <t>Aashish Sachdeva</t>
+  </si>
+  <si>
+    <t>aashish.sachdeva@sitpune.edu.un</t>
   </si>
 </sst>
 </file>
@@ -190,10 +196,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -350,12 +356,24 @@
         <v>2</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" display="aishwarya.singh@sitpune.edu.in"/>
     <hyperlink ref="C5" r:id="rId2" display="akshita.pradhan@sitpune.edu.in"/>
     <hyperlink ref="C6" r:id="rId3" display="ameya.bhattacharya@sitpune.edu.in"/>
     <hyperlink ref="C7" r:id="rId4" display="1994aishwaryasingh@gmail.com"/>
+    <hyperlink ref="C8" r:id="rId5" display="aashish.sachdeva@sitpune.edu.un"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
validation on import:role_id complete,
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -77,7 +77,7 @@
     <t>Aashish Sachdeva</t>
   </si>
   <si>
-    <t>aashish.sachdeva@sitpune.edu.un</t>
+    <t>aashishss.sachdeva@sitpune.edu.in</t>
   </si>
 </sst>
 </file>
@@ -199,7 +199,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="8:8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -342,7 +342,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>102</v>
       </c>
@@ -365,6 +365,9 @@
       </c>
       <c r="C8" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -373,7 +376,7 @@
     <hyperlink ref="C5" r:id="rId2" display="akshita.pradhan@sitpune.edu.in"/>
     <hyperlink ref="C6" r:id="rId3" display="ameya.bhattacharya@sitpune.edu.in"/>
     <hyperlink ref="C7" r:id="rId4" display="1994aishwaryasingh@gmail.com"/>
-    <hyperlink ref="C8" r:id="rId5" display="aashish.sachdeva@sitpune.edu.un"/>
+    <hyperlink ref="C8" r:id="rId5" display="aashishss.sachdeva@sitpune.edu.in"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>